<commit_message>
update metadata to fix other race definition
</commit_message>
<xml_diff>
--- a/data/aggregate_sample_metadata.xlsx
+++ b/data/aggregate_sample_metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shirleewohl/Desktop/Lessler-Lab/github/ncov-figures/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shirleewohl/Desktop/Lessler-Lab/github/jhu-covid-pipeline/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C619855-29D6-8F49-A730-297BBBFD8856}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{056B8A77-5172-B548-839F-220BB72194CC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3520" yWindow="2660" windowWidth="26920" windowHeight="17760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="aggregate_sample_metadata" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">aggregate_sample_metadata!$A$1:$E$111</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">aggregate_sample_metadata!$A$1:$E$110</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="221">
   <si>
     <t>value</t>
   </si>
@@ -1724,10 +1724,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E113"/>
+  <dimension ref="A1:E112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="A114" sqref="A114"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2318,935 +2318,935 @@
       </c>
       <c r="C39" s="15"/>
       <c r="D39" s="15" t="s">
-        <v>21</v>
+        <v>75</v>
       </c>
       <c r="E39" s="16" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="17"/>
-      <c r="B40" s="18" t="s">
+      <c r="A40" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C40" s="11"/>
+      <c r="D40" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="E40" s="12" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="13"/>
+      <c r="B41" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="C41" s="15"/>
+      <c r="D41" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="E41" s="16" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="17"/>
+      <c r="B42" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C40" s="19"/>
-      <c r="D40" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="E40" s="20" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="B41" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="C41" s="11"/>
-      <c r="D41" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="E41" s="12" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="13"/>
-      <c r="B42" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="C42" s="15"/>
-      <c r="D42" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="E42" s="16" t="s">
-        <v>108</v>
+      <c r="C42" s="19"/>
+      <c r="D42" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="E42" s="20" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" s="17"/>
-      <c r="B43" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C43" s="19"/>
-      <c r="D43" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="E43" s="20" t="s">
-        <v>41</v>
+      <c r="A43" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C43" s="11"/>
+      <c r="D43" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="E43" s="12" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="B44" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="C44" s="11"/>
-      <c r="D44" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="E44" s="12" t="s">
-        <v>78</v>
+      <c r="A44" s="13"/>
+      <c r="B44" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="C44" s="15"/>
+      <c r="D44" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="E44" s="16" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="13"/>
       <c r="B45" s="14" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C45" s="15"/>
       <c r="D45" s="15" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="E45" s="16" t="s">
-        <v>115</v>
+        <v>10</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" s="13"/>
-      <c r="B46" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="C46" s="15"/>
-      <c r="D46" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="E46" s="16" t="s">
-        <v>10</v>
+      <c r="A46" s="17"/>
+      <c r="B46" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C46" s="19"/>
+      <c r="D46" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="E46" s="20" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" s="17"/>
-      <c r="B47" s="18" t="s">
+      <c r="A47" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C47" s="11"/>
+      <c r="D47" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="E47" s="12" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="13"/>
+      <c r="B48" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="C48" s="15"/>
+      <c r="D48" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="E48" s="16" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" s="17"/>
+      <c r="B49" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C47" s="19"/>
-      <c r="D47" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="E47" s="20" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="B48" s="10" t="s">
+      <c r="C49" s="19"/>
+      <c r="D49" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="E49" s="20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="B50" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="C48" s="11"/>
-      <c r="D48" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="E48" s="12" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49" s="13"/>
-      <c r="B49" s="14" t="s">
+      <c r="C50" s="11"/>
+      <c r="D50" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="E50" s="12" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" s="13"/>
+      <c r="B51" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="C49" s="15"/>
-      <c r="D49" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="E49" s="16" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50" s="17"/>
-      <c r="B50" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C50" s="19"/>
-      <c r="D50" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="E50" s="20" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="B51" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="C51" s="11"/>
-      <c r="D51" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="E51" s="12" t="s">
-        <v>125</v>
+      <c r="C51" s="15"/>
+      <c r="D51" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="E51" s="16" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="13"/>
       <c r="B52" s="14" t="s">
-        <v>106</v>
+        <v>11</v>
       </c>
       <c r="C52" s="15"/>
       <c r="D52" s="15" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E52" s="16" t="s">
-        <v>4</v>
+        <v>51</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A53" s="13"/>
-      <c r="B53" s="14" t="s">
+      <c r="A53" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="B53" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C53" s="11"/>
+      <c r="D53" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="E53" s="12" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" s="13"/>
+      <c r="B54" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="C54" s="15"/>
+      <c r="D54" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E54" s="16" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" s="17"/>
+      <c r="B55" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C53" s="15"/>
-      <c r="D53" s="15" t="s">
+      <c r="C55" s="19"/>
+      <c r="D55" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="E53" s="16" t="s">
+      <c r="E55" s="20" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A54" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="B54" s="10" t="s">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="B56" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="C54" s="11"/>
-      <c r="D54" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="E54" s="12" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A55" s="13"/>
-      <c r="B55" s="14" t="s">
+      <c r="C56" s="11"/>
+      <c r="D56" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="E56" s="12" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" s="13"/>
+      <c r="B57" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="C55" s="15"/>
-      <c r="D55" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="E55" s="16" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A56" s="17"/>
-      <c r="B56" s="18" t="s">
+      <c r="C57" s="15"/>
+      <c r="D57" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="E57" s="16" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" s="17"/>
+      <c r="B58" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C56" s="19"/>
-      <c r="D56" s="19" t="s">
+      <c r="C58" s="19"/>
+      <c r="D58" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="E56" s="20" t="s">
+      <c r="E58" s="20" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A57" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="B57" s="10" t="s">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="B59" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="C57" s="11"/>
-      <c r="D57" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="E57" s="12" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A58" s="13"/>
-      <c r="B58" s="14" t="s">
+      <c r="C59" s="11"/>
+      <c r="D59" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="E59" s="12" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" s="13"/>
+      <c r="B60" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="C58" s="15"/>
-      <c r="D58" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="E58" s="16" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A59" s="17"/>
-      <c r="B59" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C59" s="19"/>
-      <c r="D59" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="E59" s="20" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A60" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="B60" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="C60" s="11"/>
-      <c r="D60" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="E60" s="12" t="s">
-        <v>138</v>
+      <c r="C60" s="15"/>
+      <c r="D60" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E60" s="16" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="13"/>
       <c r="B61" s="14" t="s">
-        <v>106</v>
+        <v>11</v>
       </c>
       <c r="C61" s="15"/>
       <c r="D61" s="15" t="s">
         <v>9</v>
       </c>
       <c r="E61" s="16" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="B62" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C62" s="11"/>
+      <c r="D62" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="E62" s="12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63" s="13"/>
+      <c r="B63" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="C63" s="15"/>
+      <c r="D63" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="E63" s="16" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64" s="17"/>
+      <c r="B64" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C64" s="19"/>
+      <c r="D64" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="E64" s="20" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A65" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="B65" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C65" s="11"/>
+      <c r="D65" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="E65" s="12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A66" s="13"/>
+      <c r="B66" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="C66" s="15"/>
+      <c r="D66" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="E66" s="16" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67" s="17"/>
+      <c r="B67" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C67" s="19"/>
+      <c r="D67" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="E67" s="20" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A68" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B68" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C68" s="11"/>
+      <c r="D68" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="E68" s="12" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A69" s="13"/>
+      <c r="B69" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="C69" s="15"/>
+      <c r="D69" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="E69" s="16" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A70" s="17"/>
+      <c r="B70" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C70" s="19"/>
+      <c r="D70" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="E70" s="20" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A71" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="B71" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C71" s="11"/>
+      <c r="D71" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="E71" s="12" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A72" s="13"/>
+      <c r="B72" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="C72" s="15"/>
+      <c r="D72" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="E72" s="16" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A73" s="17"/>
+      <c r="B73" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C73" s="19"/>
+      <c r="D73" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="E73" s="20" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A74" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="B74" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C74" s="11"/>
+      <c r="D74" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="E74" s="12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A75" s="13"/>
+      <c r="B75" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="C75" s="15"/>
+      <c r="D75" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="E75" s="16" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A76" s="17"/>
+      <c r="B76" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C76" s="19"/>
+      <c r="D76" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="E76" s="20" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A77" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="B77" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C77" s="11"/>
+      <c r="D77" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="E77" s="12" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A78" s="13"/>
+      <c r="B78" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="C78" s="15"/>
+      <c r="D78" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="E78" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A79" s="17"/>
+      <c r="B79" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C79" s="19"/>
+      <c r="D79" s="19" t="s">
+        <v>164</v>
+      </c>
+      <c r="E79" s="20" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A80" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="B80" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C80" s="11"/>
+      <c r="D80" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="E80" s="12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A81" s="13"/>
+      <c r="B81" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="C81" s="15"/>
+      <c r="D81" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="E81" s="16" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A82" s="17"/>
+      <c r="B82" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C82" s="19"/>
+      <c r="D82" s="19" t="s">
+        <v>164</v>
+      </c>
+      <c r="E82" s="20" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A83" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="B83" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C83" s="11"/>
+      <c r="D83" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="E83" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A84" s="13"/>
+      <c r="B84" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="C84" s="15"/>
+      <c r="D84" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E84" s="16" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A85" s="17"/>
+      <c r="B85" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C85" s="19"/>
+      <c r="D85" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="E85" s="20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A86" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="B86" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C86" s="11"/>
+      <c r="D86" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="E86" s="12" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A87" s="13"/>
+      <c r="B87" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="C87" s="15"/>
+      <c r="D87" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="E87" s="16" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A88" s="17"/>
+      <c r="B88" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C88" s="19"/>
+      <c r="D88" s="19" t="s">
+        <v>164</v>
+      </c>
+      <c r="E88" s="20" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A89" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="B89" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C89" s="11"/>
+      <c r="D89" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="E89" s="12" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A90" s="13"/>
+      <c r="B90" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="C90" s="15"/>
+      <c r="D90" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="E90" s="16" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A62" s="13"/>
-      <c r="B62" s="14" t="s">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A91" s="17"/>
+      <c r="B91" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C62" s="15"/>
-      <c r="D62" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E62" s="16" t="s">
+      <c r="C91" s="19"/>
+      <c r="D91" s="19" t="s">
+        <v>164</v>
+      </c>
+      <c r="E91" s="20" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A63" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="B63" s="10" t="s">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A92" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="B92" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="C63" s="11"/>
-      <c r="D63" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="E63" s="12" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A64" s="13"/>
-      <c r="B64" s="14" t="s">
+      <c r="C92" s="11"/>
+      <c r="D92" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="E92" s="12" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A93" s="13"/>
+      <c r="B93" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="C64" s="15"/>
-      <c r="D64" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="E64" s="16" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A65" s="17"/>
-      <c r="B65" s="18" t="s">
+      <c r="C93" s="15"/>
+      <c r="D93" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="E93" s="16" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A94" s="17"/>
+      <c r="B94" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C65" s="19"/>
-      <c r="D65" s="19" t="s">
-        <v>143</v>
-      </c>
-      <c r="E65" s="20" t="s">
+      <c r="C94" s="19"/>
+      <c r="D94" s="19" t="s">
+        <v>164</v>
+      </c>
+      <c r="E94" s="20" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A66" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="B66" s="10" t="s">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A95" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="B95" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="C66" s="11"/>
-      <c r="D66" s="11" t="s">
-        <v>145</v>
-      </c>
-      <c r="E66" s="12" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A67" s="13"/>
-      <c r="B67" s="14" t="s">
+      <c r="C95" s="11"/>
+      <c r="D95" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="E95" s="12" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A96" s="13"/>
+      <c r="B96" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="C67" s="15"/>
-      <c r="D67" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="E67" s="16" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A68" s="17"/>
-      <c r="B68" s="18" t="s">
+      <c r="C96" s="15"/>
+      <c r="D96" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="E96" s="16" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A97" s="17"/>
+      <c r="B97" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C68" s="19"/>
-      <c r="D68" s="19" t="s">
-        <v>143</v>
-      </c>
-      <c r="E68" s="20" t="s">
+      <c r="C97" s="19"/>
+      <c r="D97" s="19" t="s">
+        <v>164</v>
+      </c>
+      <c r="E97" s="20" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A69" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="B69" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="C69" s="11"/>
-      <c r="D69" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="E69" s="12" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A70" s="13"/>
-      <c r="B70" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="C70" s="15"/>
-      <c r="D70" s="15" t="s">
-        <v>150</v>
-      </c>
-      <c r="E70" s="16" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A71" s="17"/>
-      <c r="B71" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C71" s="19"/>
-      <c r="D71" s="19" t="s">
-        <v>143</v>
-      </c>
-      <c r="E71" s="20" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A72" s="9" t="s">
-        <v>152</v>
-      </c>
-      <c r="B72" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="C72" s="11"/>
-      <c r="D72" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E72" s="12" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A73" s="13"/>
-      <c r="B73" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="C73" s="15"/>
-      <c r="D73" s="15" t="s">
-        <v>155</v>
-      </c>
-      <c r="E73" s="16" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A74" s="17"/>
-      <c r="B74" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C74" s="19"/>
-      <c r="D74" s="19" t="s">
-        <v>143</v>
-      </c>
-      <c r="E74" s="20" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A75" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="B75" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="C75" s="11"/>
-      <c r="D75" s="11" t="s">
-        <v>158</v>
-      </c>
-      <c r="E75" s="12" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A76" s="13"/>
-      <c r="B76" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="C76" s="15"/>
-      <c r="D76" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="E76" s="16" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A77" s="17"/>
-      <c r="B77" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C77" s="19"/>
-      <c r="D77" s="19" t="s">
-        <v>143</v>
-      </c>
-      <c r="E77" s="20" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A78" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="B78" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="C78" s="11"/>
-      <c r="D78" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E78" s="12" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A79" s="13"/>
-      <c r="B79" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="C79" s="15"/>
-      <c r="D79" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="E79" s="16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A80" s="17"/>
-      <c r="B80" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C80" s="19"/>
-      <c r="D80" s="19" t="s">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A98" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="B98" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="C98" s="11"/>
+      <c r="D98" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="E80" s="20" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A81" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="B81" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="C81" s="11"/>
-      <c r="D81" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="E81" s="12" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A82" s="13"/>
-      <c r="B82" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="C82" s="15"/>
-      <c r="D82" s="15" t="s">
-        <v>167</v>
-      </c>
-      <c r="E82" s="16" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A83" s="17"/>
-      <c r="B83" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C83" s="19"/>
-      <c r="D83" s="19" t="s">
-        <v>164</v>
-      </c>
-      <c r="E83" s="20" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A84" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="B84" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="C84" s="11"/>
-      <c r="D84" s="11" t="s">
-        <v>169</v>
-      </c>
-      <c r="E84" s="12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A85" s="13"/>
-      <c r="B85" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="C85" s="15"/>
-      <c r="D85" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="E85" s="16" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A86" s="17"/>
-      <c r="B86" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C86" s="19"/>
-      <c r="D86" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="E86" s="20" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A87" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="B87" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="C87" s="11"/>
-      <c r="D87" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="E87" s="12" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A88" s="13"/>
-      <c r="B88" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="C88" s="15"/>
-      <c r="D88" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="E88" s="16" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A89" s="17"/>
-      <c r="B89" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C89" s="19"/>
-      <c r="D89" s="19" t="s">
-        <v>164</v>
-      </c>
-      <c r="E89" s="20" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A90" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="B90" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="C90" s="11"/>
-      <c r="D90" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="E90" s="12" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A91" s="13"/>
-      <c r="B91" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="C91" s="15"/>
-      <c r="D91" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="E91" s="16" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A92" s="17"/>
-      <c r="B92" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C92" s="19"/>
-      <c r="D92" s="19" t="s">
-        <v>164</v>
-      </c>
-      <c r="E92" s="20" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A93" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="B93" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="C93" s="11"/>
-      <c r="D93" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E93" s="12" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A94" s="13"/>
-      <c r="B94" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="C94" s="15"/>
-      <c r="D94" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="E94" s="16" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A95" s="17"/>
-      <c r="B95" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C95" s="19"/>
-      <c r="D95" s="19" t="s">
-        <v>164</v>
-      </c>
-      <c r="E95" s="20" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A96" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="B96" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="C96" s="11"/>
-      <c r="D96" s="11" t="s">
-        <v>176</v>
-      </c>
-      <c r="E96" s="12" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A97" s="13"/>
-      <c r="B97" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="C97" s="15"/>
-      <c r="D97" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="E97" s="16" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A98" s="17"/>
-      <c r="B98" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C98" s="19"/>
-      <c r="D98" s="19" t="s">
-        <v>164</v>
-      </c>
-      <c r="E98" s="20" t="s">
-        <v>139</v>
+      <c r="E98" s="12" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A99" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="B99" s="10" t="s">
-        <v>180</v>
-      </c>
-      <c r="C99" s="11"/>
-      <c r="D99" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="E99" s="12" t="s">
-        <v>37</v>
+      <c r="A99" s="13"/>
+      <c r="B99" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="C99" s="15"/>
+      <c r="D99" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="E99" s="16" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" s="13"/>
       <c r="B100" s="14" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C100" s="15"/>
       <c r="D100" s="15" t="s">
-        <v>182</v>
+        <v>143</v>
       </c>
       <c r="E100" s="16" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A101" s="13"/>
-      <c r="B101" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="C101" s="15"/>
-      <c r="D101" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="E101" s="16" t="s">
+      <c r="A101" s="17"/>
+      <c r="B101" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C101" s="19"/>
+      <c r="D101" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E101" s="20" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A102" s="17"/>
-      <c r="B102" s="18" t="s">
+      <c r="A102" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="B102" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C102" s="11"/>
+      <c r="D102" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="E102" s="12" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A103" s="13"/>
+      <c r="B103" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="C103" s="15"/>
+      <c r="D103" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="E103" s="16" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A104" s="17"/>
+      <c r="B104" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C102" s="19"/>
-      <c r="D102" s="19" t="s">
+      <c r="C104" s="19"/>
+      <c r="D104" s="19" t="s">
+        <v>164</v>
+      </c>
+      <c r="E104" s="20" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A105" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="B105" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="C105" s="11"/>
+      <c r="D105" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E102" s="20" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A103" s="9" t="s">
-        <v>184</v>
-      </c>
-      <c r="B103" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="C103" s="11"/>
-      <c r="D103" s="11" t="s">
-        <v>185</v>
-      </c>
-      <c r="E103" s="12" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A104" s="13"/>
-      <c r="B104" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="C104" s="15"/>
-      <c r="D104" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="E104" s="16" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A105" s="17"/>
-      <c r="B105" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C105" s="19"/>
-      <c r="D105" s="19" t="s">
-        <v>164</v>
-      </c>
-      <c r="E105" s="20" t="s">
-        <v>139</v>
+      <c r="E105" s="12" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A106" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="B106" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="C106" s="11"/>
-      <c r="D106" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E106" s="12" t="s">
-        <v>189</v>
+      <c r="A106" s="13"/>
+      <c r="B106" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="C106" s="15"/>
+      <c r="D106" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="E106" s="16" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" s="13"/>
       <c r="B107" s="14" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C107" s="15"/>
       <c r="D107" s="15" t="s">
-        <v>122</v>
+        <v>40</v>
       </c>
       <c r="E107" s="16" t="s">
         <v>191</v>
@@ -3255,57 +3255,44 @@
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" s="13"/>
       <c r="B108" s="14" t="s">
-        <v>192</v>
+        <v>8</v>
       </c>
       <c r="C108" s="15"/>
       <c r="D108" s="15" t="s">
         <v>40</v>
       </c>
       <c r="E108" s="16" t="s">
-        <v>191</v>
+        <v>41</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" s="13"/>
       <c r="B109" s="14" t="s">
-        <v>8</v>
+        <v>193</v>
       </c>
       <c r="C109" s="15"/>
       <c r="D109" s="15" t="s">
-        <v>40</v>
+        <v>169</v>
       </c>
       <c r="E109" s="16" t="s">
-        <v>41</v>
+        <v>194</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A110" s="13"/>
-      <c r="B110" s="14" t="s">
-        <v>193</v>
-      </c>
-      <c r="C110" s="15"/>
-      <c r="D110" s="15" t="s">
-        <v>169</v>
-      </c>
-      <c r="E110" s="16" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A111" s="17"/>
-      <c r="B111" s="18" t="s">
+      <c r="A110" s="17"/>
+      <c r="B110" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C111" s="19"/>
-      <c r="D111" s="19" t="s">
+      <c r="C110" s="19"/>
+      <c r="D110" s="19" t="s">
         <v>164</v>
       </c>
-      <c r="E111" s="20" t="s">
+      <c r="E110" s="20" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A113" s="2" t="s">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A112" s="2" t="s">
         <v>220</v>
       </c>
     </row>

</xml_diff>